<commit_message>
added test plan and updated bug list
</commit_message>
<xml_diff>
--- a/doc/bug_report.xlsx
+++ b/doc/bug_report.xlsx
@@ -497,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -556,6 +556,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -1235,8 +1238,8 @@
       <c r="D10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>14</v>
+      <c r="E10" s="21" t="s">
+        <v>22</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>39</v>
@@ -1273,34 +1276,34 @@
       <c r="Z10" s="5"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="21">
+      <c r="A11" s="22">
         <v>8.0</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="23">
         <v>45354.0</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="J11" s="26" t="s">
         <v>48</v>
       </c>
       <c r="K11" s="6"/>
@@ -1321,34 +1324,34 @@
       <c r="Z11" s="5"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="21">
+      <c r="A12" s="22">
         <v>9.0</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="23">
         <v>45354.0</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>14</v>
+      <c r="E12" s="22" t="s">
+        <v>22</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="27" t="s">
         <v>52</v>
       </c>
       <c r="K12" s="6"/>
@@ -1369,37 +1372,37 @@
       <c r="Z12" s="5"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="21">
+      <c r="A13" s="22">
         <v>10.0</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="23">
         <v>45353.0</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="I13" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="25" t="s">
+      <c r="J13" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="K13" s="28"/>
+      <c r="K13" s="29"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -1417,37 +1420,37 @@
       <c r="Z13" s="5"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="21">
+      <c r="A14" s="22">
         <v>11.0</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="23">
         <v>45356.0</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="21" t="s">
-        <v>14</v>
+      <c r="E14" s="22" t="s">
+        <v>22</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="I14" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="K14" s="28"/>
+      <c r="K14" s="29"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
@@ -1465,34 +1468,34 @@
       <c r="Z14" s="5"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="21">
+      <c r="A15" s="22">
         <v>12.0</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="23">
         <v>45356.0</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>14</v>
+      <c r="E15" s="22" t="s">
+        <v>22</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="25" t="s">
+      <c r="I15" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="30"/>
+      <c r="J15" s="31"/>
       <c r="K15" s="6"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -1511,37 +1514,37 @@
       <c r="Z15" s="5"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="21">
+      <c r="A16" s="22">
         <v>13.0</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="23">
         <v>45356.0</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="25" t="s">
+      <c r="I16" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="24" t="s">
+      <c r="K16" s="25" t="s">
         <v>69</v>
       </c>
       <c r="L16" s="5"/>
@@ -1561,37 +1564,37 @@
       <c r="Z16" s="5"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="31">
+      <c r="A17" s="32">
         <v>14.0</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="33">
         <v>45356.0</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="33" t="s">
-        <v>14</v>
+      <c r="E17" s="34" t="s">
+        <v>22</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="34" t="s">
+      <c r="G17" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="H17" s="34" t="s">
+      <c r="H17" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="I17" s="34" t="s">
+      <c r="I17" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="34" t="s">
+      <c r="J17" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="K17" s="35"/>
+      <c r="K17" s="36"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
@@ -1609,34 +1612,34 @@
       <c r="Z17" s="5"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="36">
+      <c r="A18" s="37">
         <v>15.0</v>
       </c>
-      <c r="B18" s="32">
+      <c r="B18" s="33">
         <v>45377.0</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="H18" s="36" t="s">
+      <c r="H18" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="I18" s="36" t="s">
+      <c r="I18" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="J18" s="36" t="s">
+      <c r="J18" s="37" t="s">
         <v>78</v>
       </c>
       <c r="L18" s="5"/>
@@ -1656,34 +1659,34 @@
       <c r="Z18" s="5"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="36">
+      <c r="A19" s="37">
         <v>16.0</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="33">
         <v>45377.0</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="36" t="s">
+      <c r="F19" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="H19" s="36" t="s">
+      <c r="H19" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="I19" s="36" t="s">
+      <c r="I19" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="J19" s="36" t="s">
+      <c r="J19" s="37" t="s">
         <v>83</v>
       </c>
       <c r="L19" s="5"/>
@@ -1703,34 +1706,34 @@
       <c r="Z19" s="5"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="37">
+      <c r="A20" s="38">
         <v>17.0</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="33">
         <v>45377.0</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="36" t="s">
+      <c r="E20" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="I20" s="36" t="s">
+      <c r="I20" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="J20" s="36" t="s">
+      <c r="J20" s="37" t="s">
         <v>87</v>
       </c>
       <c r="L20" s="5"/>
@@ -1750,34 +1753,34 @@
       <c r="Z20" s="5"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="37">
+      <c r="A21" s="38">
         <v>18.0</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="33">
         <v>45377.0</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="F21" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="I21" s="36" t="s">
+      <c r="I21" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="J21" s="36" t="s">
+      <c r="J21" s="37" t="s">
         <v>92</v>
       </c>
       <c r="L21" s="5"/>
@@ -1797,37 +1800,37 @@
       <c r="Z21" s="5"/>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="36">
+      <c r="A22" s="37">
         <v>19.0</v>
       </c>
-      <c r="B22" s="32">
+      <c r="B22" s="33">
         <v>45377.0</v>
       </c>
-      <c r="C22" s="36" t="s">
+      <c r="C22" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="36" t="s">
+      <c r="F22" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="H22" s="36" t="s">
+      <c r="H22" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="I22" s="36" t="s">
+      <c r="I22" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="J22" s="36" t="s">
+      <c r="J22" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="K22" s="36" t="s">
+      <c r="K22" s="37" t="s">
         <v>97</v>
       </c>
       <c r="L22" s="5"/>
@@ -1847,37 +1850,37 @@
       <c r="Z22" s="5"/>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="21">
+      <c r="A23" s="22">
         <v>20.0</v>
       </c>
-      <c r="B23" s="32">
+      <c r="B23" s="33">
         <v>45377.0</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D23" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="F23" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="25" t="s">
+      <c r="G23" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="I23" s="25" t="s">
+      <c r="I23" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="J23" s="25" t="s">
+      <c r="J23" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="K23" s="24" t="s">
+      <c r="K23" s="25" t="s">
         <v>101</v>
       </c>
       <c r="L23" s="5"/>
@@ -1897,34 +1900,34 @@
       <c r="Z23" s="5"/>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="21">
+      <c r="A24" s="22">
         <v>21.0</v>
       </c>
-      <c r="B24" s="32">
+      <c r="B24" s="33">
         <v>45377.0</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="E24" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="H24" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="I24" s="25" t="s">
+      <c r="I24" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="J24" s="25" t="s">
+      <c r="J24" s="26" t="s">
         <v>104</v>
       </c>
       <c r="K24" s="6"/>
@@ -1945,34 +1948,34 @@
       <c r="Z24" s="5"/>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="21">
+      <c r="A25" s="22">
         <v>22.0</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="23">
         <v>45378.0</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="G25" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="H25" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="I25" s="25" t="s">
+      <c r="I25" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="J25" s="25" t="s">
+      <c r="J25" s="26" t="s">
         <v>108</v>
       </c>
       <c r="K25" s="6"/>
@@ -1993,37 +1996,37 @@
       <c r="Z25" s="5"/>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="21">
+      <c r="A26" s="22">
         <v>23.0</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="23">
         <v>45378.0</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="38" t="s">
+      <c r="G26" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="H26" s="25" t="s">
+      <c r="H26" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="I26" s="38" t="s">
+      <c r="I26" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="J26" s="25" t="s">
+      <c r="J26" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="K26" s="26" t="s">
+      <c r="K26" s="27" t="s">
         <v>112</v>
       </c>
       <c r="L26" s="5"/>
@@ -2043,7 +2046,7 @@
       <c r="Z26" s="5"/>
     </row>
     <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="39"/>
+      <c r="A27" s="40"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -2071,8 +2074,8 @@
       <c r="Z27" s="5"/>
     </row>
     <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="40"/>
-      <c r="B28" s="41"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="42"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -2099,8 +2102,8 @@
       <c r="Z28" s="5"/>
     </row>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="41"/>
-      <c r="B29" s="41"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -2127,8 +2130,8 @@
       <c r="Z29" s="5"/>
     </row>
     <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
@@ -2155,8 +2158,8 @@
       <c r="Z30" s="5"/>
     </row>
     <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="42"/>
-      <c r="B31" s="41"/>
+      <c r="A31" s="43"/>
+      <c r="B31" s="42"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
@@ -2183,8 +2186,8 @@
       <c r="Z31" s="5"/>
     </row>
     <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="41"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="42"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
@@ -29335,58 +29338,58 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="44" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="44" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="44" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="44" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="44" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="44" t="s">
         <v>122</v>
       </c>
     </row>

</xml_diff>